<commit_message>
Formatted H&M Template a bit
</commit_message>
<xml_diff>
--- a/Honey & Mumford Template.xlsx
+++ b/Honey & Mumford Template.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OpenSource\PersonalityQuestionnaires\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Documents\PersonalityQuestionnaires\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{53C50B5D-64BC-45ED-A368-6FE528D9CF9F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E3CA3D57-239D-4D85-8D2E-474CD14AA376}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9660" activeTab="1" xr2:uid="{F81B07BC-F333-4C43-A608-74C7104E2B79}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9660" xr2:uid="{F81B07BC-F333-4C43-A608-74C7104E2B79}"/>
   </bookViews>
   <sheets>
     <sheet name="Questions" sheetId="2" r:id="rId1"/>
     <sheet name="Outcome" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -357,7 +357,51 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -368,6 +412,17 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{352F1A96-64AE-47A2-BC10-DA115014BFE2}" name="Table1" displayName="Table1" ref="A1:B81" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:B81" xr:uid="{82266221-8D7A-404B-BB69-4A8363A9287B}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{D1FAC0EC-23E4-4EB0-B425-5A9A899781CF}" name="Answer" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{7048DE7F-D6A0-48E9-9BBD-323C755930BD}" name="Question"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -669,17 +724,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4BF6E2F-A576-4BF8-93D8-FC03F976B271}">
   <dimension ref="A1:B81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="3"/>
-    <col min="2" max="2" width="13.77734375" customWidth="1"/>
+    <col min="1" max="1" width="2" style="3" customWidth="1"/>
+    <col min="2" max="2" width="113.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -687,7 +742,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -695,7 +750,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>0</v>
       </c>
@@ -703,7 +758,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>0</v>
       </c>
@@ -711,7 +766,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>0</v>
       </c>
@@ -719,7 +774,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>0</v>
       </c>
@@ -727,7 +782,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>0</v>
       </c>
@@ -735,7 +790,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>0</v>
       </c>
@@ -743,7 +798,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>0</v>
       </c>
@@ -751,7 +806,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>0</v>
       </c>
@@ -759,7 +814,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>0</v>
       </c>
@@ -767,7 +822,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>0</v>
       </c>
@@ -775,7 +830,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>0</v>
       </c>
@@ -783,7 +838,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>0</v>
       </c>
@@ -791,7 +846,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>0</v>
       </c>
@@ -799,7 +854,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>0</v>
       </c>
@@ -807,7 +862,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>0</v>
       </c>
@@ -815,7 +870,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>0</v>
       </c>
@@ -823,7 +878,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>0</v>
       </c>
@@ -831,7 +886,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>0</v>
       </c>
@@ -839,7 +894,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>0</v>
       </c>
@@ -847,7 +902,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>0</v>
       </c>
@@ -855,7 +910,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>0</v>
       </c>
@@ -863,7 +918,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>0</v>
       </c>
@@ -871,7 +926,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>0</v>
       </c>
@@ -879,7 +934,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>0</v>
       </c>
@@ -887,7 +942,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>0</v>
       </c>
@@ -895,7 +950,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>0</v>
       </c>
@@ -903,7 +958,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>0</v>
       </c>
@@ -911,7 +966,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>0</v>
       </c>
@@ -919,7 +974,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>0</v>
       </c>
@@ -927,7 +982,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>0</v>
       </c>
@@ -935,7 +990,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>0</v>
       </c>
@@ -943,7 +998,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>0</v>
       </c>
@@ -951,7 +1006,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>0</v>
       </c>
@@ -959,7 +1014,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>0</v>
       </c>
@@ -967,7 +1022,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>0</v>
       </c>
@@ -975,7 +1030,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>0</v>
       </c>
@@ -983,7 +1038,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>0</v>
       </c>
@@ -991,7 +1046,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>0</v>
       </c>
@@ -999,7 +1054,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>0</v>
       </c>
@@ -1007,7 +1062,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>0</v>
       </c>
@@ -1015,7 +1070,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>0</v>
       </c>
@@ -1023,7 +1078,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>0</v>
       </c>
@@ -1031,7 +1086,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>0</v>
       </c>
@@ -1039,7 +1094,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>0</v>
       </c>
@@ -1047,7 +1102,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>0</v>
       </c>
@@ -1055,7 +1110,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>0</v>
       </c>
@@ -1063,7 +1118,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>0</v>
       </c>
@@ -1071,7 +1126,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>0</v>
       </c>
@@ -1079,7 +1134,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>0</v>
       </c>
@@ -1087,7 +1142,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>0</v>
       </c>
@@ -1095,7 +1150,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>0</v>
       </c>
@@ -1103,7 +1158,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>0</v>
       </c>
@@ -1111,7 +1166,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>0</v>
       </c>
@@ -1119,7 +1174,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>0</v>
       </c>
@@ -1127,7 +1182,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>0</v>
       </c>
@@ -1135,7 +1190,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>0</v>
       </c>
@@ -1143,7 +1198,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>0</v>
       </c>
@@ -1151,7 +1206,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>0</v>
       </c>
@@ -1159,7 +1214,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>0</v>
       </c>
@@ -1167,7 +1222,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>0</v>
       </c>
@@ -1175,7 +1230,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>0</v>
       </c>
@@ -1183,7 +1238,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>0</v>
       </c>
@@ -1191,7 +1246,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>0</v>
       </c>
@@ -1199,7 +1254,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>0</v>
       </c>
@@ -1207,7 +1262,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>0</v>
       </c>
@@ -1215,7 +1270,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>0</v>
       </c>
@@ -1223,7 +1278,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>0</v>
       </c>
@@ -1231,7 +1286,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>0</v>
       </c>
@@ -1239,7 +1294,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>0</v>
       </c>
@@ -1247,7 +1302,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>0</v>
       </c>
@@ -1255,7 +1310,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>0</v>
       </c>
@@ -1263,7 +1318,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>0</v>
       </c>
@@ -1271,7 +1326,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>0</v>
       </c>
@@ -1279,7 +1334,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>0</v>
       </c>
@@ -1287,7 +1342,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>0</v>
       </c>
@@ -1295,7 +1350,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>0</v>
       </c>
@@ -1303,7 +1358,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>0</v>
       </c>
@@ -1311,7 +1366,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>0</v>
       </c>
@@ -1319,7 +1374,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>0</v>
       </c>
@@ -1329,6 +1384,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1336,20 +1394,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD1B4296-D68F-40AA-A935-AFB247084132}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" customWidth="1"/>
-    <col min="3" max="3" width="15.21875" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1366,7 +1424,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1387,7 +1445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3">
         <f>Questions!A3</f>
         <v>0</v>
@@ -1405,7 +1463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4">
         <f>Questions!A5</f>
         <v>0</v>
@@ -1423,7 +1481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5">
         <f>Questions!A7</f>
         <v>0</v>
@@ -1441,7 +1499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6">
         <f>Questions!A11</f>
         <v>0</v>
@@ -1459,7 +1517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7">
         <f>Questions!A18</f>
         <v>0</v>
@@ -1477,7 +1535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8">
         <f>Questions!A24</f>
         <v>0</v>
@@ -1495,7 +1553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9">
         <f>Questions!A25</f>
         <v>0</v>
@@ -1513,7 +1571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10">
         <f>Questions!A33</f>
         <v>0</v>
@@ -1531,7 +1589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11">
         <f>Questions!A35</f>
         <v>0</v>
@@ -1549,7 +1607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12">
         <f>Questions!A39</f>
         <v>0</v>
@@ -1567,7 +1625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13">
         <f>Questions!A41</f>
         <v>0</v>
@@ -1585,7 +1643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14">
         <f>Questions!A44</f>
         <v>0</v>
@@ -1603,7 +1661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15">
         <f>Questions!A46</f>
         <v>0</v>
@@ -1621,7 +1679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16">
         <f>Questions!A49</f>
         <v>0</v>
@@ -1639,7 +1697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17">
         <f>Questions!A60</f>
         <v>0</v>
@@ -1657,7 +1715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18">
         <f>Questions!A67</f>
         <v>0</v>
@@ -1675,7 +1733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19">
         <f>Questions!A74</f>
         <v>0</v>
@@ -1693,7 +1751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20">
         <f>Questions!A75</f>
         <v>0</v>
@@ -1711,7 +1769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21">
         <f>Questions!A77</f>
         <v>0</v>
@@ -1729,7 +1787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22">
         <f>Questions!A82</f>
         <v>0</v>

</xml_diff>